<commit_message>
added test 'create invalid computer' added readme
</commit_message>
<xml_diff>
--- a/ManualTests.xlsx
+++ b/ManualTests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\webtest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C62C9D1A-FDC1-4D0F-A2AA-D0CFEE66580B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4C3B23B7-AB25-41C7-9258-8483CD0AC5BB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{0689189E-0D20-41CF-87AA-C6D22A2D9CD3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="108">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -206,13 +206,300 @@
   </si>
   <si>
     <t>2015-11-30</t>
+  </si>
+  <si>
+    <t>ToDo:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Acceptance criteria: null values are saved fine.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    (Actual result: pass)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Acceptance criteria: fail on creating second computer. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    (Actual result: fail)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Acceptance criteria: no reaction on injections.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    (Was tested with </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        &lt;script&gt; function myFunc(){alert("alert");}&lt;/script&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        - passed) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Acceptance criteria: document would be created and found.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    (Actual result: failed. Document was not found)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Acceptance criteria: create/edit fails.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    (Actual resultL failed. It is possible to create/edit computer with this condition)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Acceptance criteria: create/edit computer fails.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Acceptance criteria: search filter should be cut on error should be generated like wrong search filter.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    (Actual result: server fails with application error.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Acceptance criteria: name be cut to reasonable number of symbols on error should be generated like: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "wrong computer name. Max length is 64 symbols."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    (Actual result: server fails with application error)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    -&gt; For this test need more implementation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Acceptance criteria: data is filters as expected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Acceptance criteria: correct info in info bar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Acceptance criteria: arrow are greyed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Acceptance criteria: main page is shown with any filter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    (Actual result pass)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Acceptance criteria: date is parsed correct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    -&gt; For this test need to improve error handler on parsing date and implement random date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    for computers.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    (Actual result is pass)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Null values on edit Computer.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">Add test with creating same computers (2 same computers). </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">Add test with adding vulnerabilities check (sql injection,cross site scripting.) on edit computer. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">Create/Edit computer where introduced date is less then discontinued date. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">Put date with wrong format on edit. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">Do search by large string (increase from 256 symbols to 4096). </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Create document with large string in name</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">Filter data (by Computer name/Introduced/Discontinued/Company). </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="204"/>
+      </rPr>
+      <t>List Pages and Check if number of shown PC = info in status bar</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Check that arrow are grayed in first last pages</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Clicking on 'Play sample application — Computer database' return on main page.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Check that date is parsed correct</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Edit Computer feature</t>
+  </si>
+  <si>
+    <t>Also add following cases:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Search Computer feature</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Sort List feature</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Delete Computer feature</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Working with List feature</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">Create computer with special symbols (like: ~!@#$%^&amp;*()_+). </t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,6 +522,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="3">
@@ -310,50 +610,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -394,6 +652,54 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -711,9 +1017,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0241181-99E7-4DE7-B26F-335C645ADB50}">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -731,737 +1039,1037 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="5" t="s">
+      <c r="G2" s="1"/>
+      <c r="H2" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="15"/>
-      <c r="K2" s="11"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="24"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="14" t="s">
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="5"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="11"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="24"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="15" t="s">
+      <c r="A4" s="22"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H4" s="5"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="11"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="24"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="15" t="s">
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H5" s="5"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="11"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="24"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="15" t="s">
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="5"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="11"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="24"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="19" t="s">
+      <c r="A7" s="22"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="15"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="11"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="24"/>
     </row>
     <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="7" t="s">
+      <c r="A8" s="22"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="17" t="s">
+      <c r="H8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="11"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="24"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="21" t="s">
+      <c r="A9" s="23"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="21"/>
-      <c r="H9" s="22" t="s">
+      <c r="G9" s="7"/>
+      <c r="H9" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="12"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="25"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="26" t="s">
+      <c r="F10" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="26"/>
-      <c r="H10" s="4" t="s">
+      <c r="G10" s="12"/>
+      <c r="H10" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I10" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="19" t="s">
+      <c r="A11" s="22"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="19" t="s">
+      <c r="A12" s="22"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="F12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G12" s="15"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
     </row>
     <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="7" t="s">
+      <c r="A13" s="22"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="F13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="15" t="s">
+      <c r="G13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H13" s="17" t="s">
+      <c r="H13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I13" s="5"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
     </row>
     <row r="14" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="21" t="s">
+      <c r="A14" s="23"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="21"/>
-      <c r="H14" s="22" t="s">
+      <c r="G14" s="7"/>
+      <c r="H14" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="I14" s="6"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="24" t="s">
+      <c r="E15" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="26" t="s">
+      <c r="F15" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="G15" s="26"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="26"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="7" t="s">
+      <c r="A16" s="22"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="15" t="s">
+      <c r="F16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G16" s="15" t="s">
+      <c r="G16" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="15" t="s">
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G17" s="15" t="s">
+      <c r="G17" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="15" t="s">
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G18" s="15" t="s">
+      <c r="G18" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
     </row>
     <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="27" t="s">
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F19" s="21" t="s">
+      <c r="F19" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21" t="s">
+      <c r="G19" s="7"/>
+      <c r="H19" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="I19" s="21" t="s">
+      <c r="I19" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="J19" s="21"/>
-      <c r="K19" s="21"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
     </row>
     <row r="20" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="E20" s="19" t="s">
+      <c r="E20" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F20" s="15" t="s">
+      <c r="F20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="7" t="s">
+      <c r="A21" s="22"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="F21" s="15" t="s">
+      <c r="F21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G21" s="15" t="s">
+      <c r="G21" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="15" t="s">
+      <c r="A22" s="22"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G22" s="29" t="s">
+      <c r="G22" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="15" t="s">
+      <c r="A23" s="22"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G23" s="15" t="s">
+      <c r="G23" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="15" t="s">
+      <c r="A24" s="22"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G24" s="15" t="s">
+      <c r="G24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
     </row>
     <row r="25" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="27" t="s">
+      <c r="A25" s="23"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F25" s="21" t="s">
+      <c r="F25" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21" t="s">
+      <c r="G25" s="7"/>
+      <c r="H25" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="I25" s="30" t="s">
+      <c r="I25" s="16" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="E26" s="19" t="s">
+      <c r="E26" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F26" s="15" t="s">
+      <c r="F26" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="7" t="s">
+      <c r="A27" s="22"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="F27" s="15" t="s">
+      <c r="F27" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G27" s="15" t="s">
+      <c r="G27" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H27" s="15"/>
-      <c r="I27" s="15"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="15" t="s">
+      <c r="A28" s="22"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G28" s="29" t="s">
+      <c r="G28" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="15" t="s">
+      <c r="A29" s="22"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G29" s="15" t="s">
+      <c r="G29" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="15" t="s">
+      <c r="A30" s="22"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G30" s="15" t="s">
+      <c r="G30" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H30" s="15"/>
-      <c r="I30" s="15"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
     </row>
     <row r="31" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="27" t="s">
+      <c r="A31" s="23"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F31" s="21" t="s">
+      <c r="F31" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21" t="s">
+      <c r="G31" s="7"/>
+      <c r="H31" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="I31" s="30" t="s">
+      <c r="I31" s="16" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="E32" s="19" t="s">
+      <c r="E32" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F32" s="15" t="s">
+      <c r="F32" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G32" s="15"/>
-      <c r="H32" s="15"/>
-      <c r="I32" s="15"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="7" t="s">
+      <c r="A33" s="22"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="F33" s="15" t="s">
+      <c r="F33" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G33" s="15" t="s">
+      <c r="G33" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H33" s="15"/>
-      <c r="I33" s="15"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="15" t="s">
+      <c r="A34" s="22"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G34" s="15" t="s">
+      <c r="G34" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H34" s="15"/>
-      <c r="I34" s="15"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="15" t="s">
+      <c r="A35" s="22"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G35" s="15" t="s">
+      <c r="G35" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H35" s="15"/>
-      <c r="I35" s="15"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="15" t="s">
+      <c r="A36" s="22"/>
+      <c r="B36" s="22"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G36" s="15" t="s">
+      <c r="G36" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H36" s="15"/>
-      <c r="I36" s="15"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="19" t="s">
+      <c r="A37" s="22"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F37" s="15" t="s">
+      <c r="F37" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G37" s="15"/>
-      <c r="H37" s="20" t="s">
+      <c r="G37" s="1"/>
+      <c r="H37" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I37" s="31" t="s">
+      <c r="I37" s="17" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="21"/>
-      <c r="B38" s="21"/>
-      <c r="C38" s="21"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="27" t="s">
+      <c r="A38" s="7"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="F38" s="21"/>
-      <c r="G38" s="21"/>
-      <c r="H38" s="28" t="s">
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="I38" s="30" t="s">
+      <c r="I38" s="16" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="33" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="33" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="33" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="33" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="33" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="33" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="32"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="33" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="33" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="32" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="32" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="33" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="33" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="32" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="32" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="33" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="32" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="32" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="33" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="32" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="33" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="32" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="32" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="33" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="32" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="32" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="33" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="32" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="32" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="33" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="32" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="32" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="33" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="32" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="32" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="32" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="33" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="32" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="32" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="32" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="33" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="32" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="32" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="33" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="32" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="32" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="32" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="A32:A37"/>
+    <mergeCell ref="B32:B37"/>
+    <mergeCell ref="C32:C37"/>
+    <mergeCell ref="D32:D37"/>
+    <mergeCell ref="E33:E36"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="C10:C14"/>
+    <mergeCell ref="B15:B19"/>
+    <mergeCell ref="C15:C19"/>
+    <mergeCell ref="D15:D19"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="E21:E24"/>
+    <mergeCell ref="B20:B25"/>
+    <mergeCell ref="C20:C25"/>
+    <mergeCell ref="D20:D25"/>
+    <mergeCell ref="A20:A25"/>
+    <mergeCell ref="A26:A31"/>
+    <mergeCell ref="B26:B31"/>
+    <mergeCell ref="C26:C31"/>
+    <mergeCell ref="D26:D31"/>
+    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="E16:E18"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="I10:I14"/>
+    <mergeCell ref="D10:D14"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="H10:H12"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="C2:C9"/>
     <mergeCell ref="D2:D9"/>
@@ -1471,33 +2079,6 @@
     <mergeCell ref="H2:H7"/>
     <mergeCell ref="I2:I7"/>
     <mergeCell ref="E3:E6"/>
-    <mergeCell ref="E16:E18"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="I10:I14"/>
-    <mergeCell ref="D10:D14"/>
-    <mergeCell ref="B10:B14"/>
-    <mergeCell ref="H10:H12"/>
-    <mergeCell ref="A26:A31"/>
-    <mergeCell ref="B26:B31"/>
-    <mergeCell ref="C26:C31"/>
-    <mergeCell ref="D26:D31"/>
-    <mergeCell ref="E27:E30"/>
-    <mergeCell ref="E21:E24"/>
-    <mergeCell ref="B20:B25"/>
-    <mergeCell ref="C20:C25"/>
-    <mergeCell ref="D20:D25"/>
-    <mergeCell ref="A20:A25"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="C10:C14"/>
-    <mergeCell ref="B15:B19"/>
-    <mergeCell ref="C15:C19"/>
-    <mergeCell ref="D15:D19"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="A32:A37"/>
-    <mergeCell ref="B32:B37"/>
-    <mergeCell ref="C32:C37"/>
-    <mergeCell ref="D32:D37"/>
-    <mergeCell ref="E33:E36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>